<commit_message>
Message Patient:Expanded message patient page objects, added tests
</commit_message>
<xml_diff>
--- a/LogBox20220513/resources/testDataInput/logBoxUserAccounts.xlsx
+++ b/LogBox20220513/resources/testDataInput/logBoxUserAccounts.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LogBoxAutomationProject\LogBoxPremiumAutomation\LogBox20220513\src\test\java\resources\excelData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LogBoxAutomationProject\LogBoxPremiumAutomation\LogBox20220513\resources\testDataInput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEB88F05-4B7F-4368-9C25-1A8425546ACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0E26584-B633-4144-AFDD-837BBBE658F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
   <si>
     <t>Username</t>
   </si>
@@ -56,13 +56,19 @@
   </si>
   <si>
     <t>preAdmissionAdmissionDischarges</t>
+  </si>
+  <si>
+    <t>messagePatient</t>
+  </si>
+  <si>
+    <t>messagepatient@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,6 +80,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -100,10 +112,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -385,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,8 +444,23 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{35BA7F48-1EDC-4882-AD86-E26A483119B5}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>